<commit_message>
Updated test cases for Sprint 1 stories.
</commit_message>
<xml_diff>
--- a/TestCases/Print Appointment Tests.xlsx
+++ b/TestCases/Print Appointment Tests.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -51,8 +51,22 @@
 2. Print the appointment.</t>
   </si>
   <si>
+    <t>PrintApp.002</t>
+  </si>
+  <si>
+    <t>Verify that staff members can print the appointment calendars by day.</t>
+  </si>
+  <si>
+    <t>1. Log in as a staff member and access the print calendar page.
+2. Attempt to print the calendar.</t>
+  </si>
+  <si>
     <t>2.a. The applicant should be able to successfully print out their appointment.
-2.b. The print out should contain the following information: Location, Time, Date, Office Address, Office Number, User's Name, User's Number, User's Email</t>
+2.b. The print out should contain the following information: Location, Time, Date, Office Address, Office Number, User's Name, User's Number, User's Email, and a default set of instructions.</t>
+  </si>
+  <si>
+    <t>2.a. The calendar for the day should be printed successfully.
+2.b. The print out should contain the following information: Location, Office Address, Applicant's Name, Applicant's Phone Number, Applicant's Email, Appointment Date, Appointment Time, and a default set of instructions.</t>
   </si>
 </sst>
 </file>
@@ -443,10 +457,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="27.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -474,7 +488,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -485,7 +499,21 @@
         <v>7</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>8</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>